<commit_message>
fix: create new bug, fix later
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\excel_to_ipxact\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beribeli/Workspace/RustroverProjects/irgen_rs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCBA8DBC-0533-4F34-A5D9-467AB976F31E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9BE66A2-719B-B34B-9BEE-A95A3F4A1297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{CE17D36E-8982-7C47-A020-5E6655990FA9}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17240" activeTab="2" xr2:uid="{CE17D36E-8982-7C47-A020-5E6655990FA9}"/>
   </bookViews>
   <sheets>
     <sheet name="version" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="53">
   <si>
     <t>BLOCK</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -244,6 +244,10 @@
   </si>
   <si>
     <t>reserved</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>regc{n}, n=0~3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -251,7 +255,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -290,7 +294,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -298,9 +302,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -646,56 +647,56 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="12.81640625" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="3"/>
+      <c r="B6" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -712,15 +713,15 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -734,7 +735,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -745,7 +746,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -766,23 +767,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08ACDB31-7888-5646-9BBF-168BB80551E6}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="7.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -808,7 +809,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -831,11 +832,11 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:8">
+      <c r="A3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -854,9 +855,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
+    <row r="4" spans="1:8">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
       <c r="C4" s="1" t="s">
         <v>38</v>
       </c>
@@ -873,9 +874,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
+    <row r="5" spans="1:8">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
       <c r="C5" s="1" t="s">
         <v>51</v>
       </c>
@@ -892,9 +893,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
+    <row r="6" spans="1:8">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
       <c r="C6" s="1" t="s">
         <v>29</v>
       </c>
@@ -911,7 +912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -934,7 +935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -957,7 +958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
         <v>41</v>
       </c>
@@ -980,11 +981,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:8">
+      <c r="A10" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1003,9 +1004,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
+    <row r="11" spans="1:8">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
       <c r="C11" s="1" t="s">
         <v>29</v>
       </c>
@@ -1037,25 +1038,25 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89FF57BE-6DA6-9A46-A269-C97099FCCA20}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="7.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1081,7 +1082,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -1104,11 +1105,11 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:8">
+      <c r="A3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1127,9 +1128,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
+    <row r="4" spans="1:8">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
       <c r="C4" s="1" t="s">
         <v>38</v>
       </c>
@@ -1146,9 +1147,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
+    <row r="5" spans="1:8">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
       <c r="C5" s="1" t="s">
         <v>51</v>
       </c>
@@ -1165,9 +1166,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
+    <row r="6" spans="1:8">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
       <c r="C6" s="1" t="s">
         <v>29</v>
       </c>
@@ -1184,7 +1185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -1207,7 +1208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -1230,7 +1231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
         <v>41</v>
       </c>
@@ -1253,11 +1254,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:8">
+      <c r="A10" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1276,9 +1277,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
+    <row r="11" spans="1:8">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
       <c r="C11" s="1" t="s">
         <v>29</v>
       </c>
@@ -1295,12 +1296,56 @@
         <v>0</v>
       </c>
     </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="1">
+        <v>16</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="1">
+        <v>16</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="A3:A6"/>
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:B11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix: find bug in register
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beribeli/Workspace/RustroverProjects/irgen_rs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9BE66A2-719B-B34B-9BEE-A95A3F4A1297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CFA7BE2-2BB8-9945-B04B-F25D9CF79DEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17240" activeTab="2" xr2:uid="{CE17D36E-8982-7C47-A020-5E6655990FA9}"/>
+    <workbookView xWindow="9140" yWindow="4520" windowWidth="20700" windowHeight="13080" activeTab="3" xr2:uid="{CE17D36E-8982-7C47-A020-5E6655990FA9}"/>
   </bookViews>
   <sheets>
     <sheet name="version" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="54">
   <si>
     <t>BLOCK</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -248,6 +248,10 @@
   </si>
   <si>
     <t>regc{n}, n=0~3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x30</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -767,7 +771,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08ACDB31-7888-5646-9BBF-168BB80551E6}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -1040,8 +1044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89FF57BE-6DA6-9A46-A269-C97099FCCA20}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -1298,7 +1302,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="3" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
fix: export regvue json but some issue in parser with ipxact
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beribeli/Workspace/RustroverProjects/irgen_rs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\irgen-rs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CFA7BE2-2BB8-9945-B04B-F25D9CF79DEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEDECE09-75B4-418D-A674-4D571F8861F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9140" yWindow="4520" windowWidth="20700" windowHeight="13080" activeTab="3" xr2:uid="{CE17D36E-8982-7C47-A020-5E6655990FA9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{CE17D36E-8982-7C47-A020-5E6655990FA9}"/>
   </bookViews>
   <sheets>
     <sheet name="version" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="55">
   <si>
     <t>BLOCK</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -243,15 +243,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>reserved</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>regc{n}, n=0~3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>0x30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reserved1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reserved0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -259,7 +263,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -651,12 +655,12 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+    <col min="1" max="1" width="12.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>45</v>
       </c>
@@ -664,7 +668,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -672,7 +676,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -680,7 +684,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -688,7 +692,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -696,7 +700,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -717,15 +721,15 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6328125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -739,7 +743,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -750,7 +754,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -771,23 +775,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08ACDB31-7888-5646-9BBF-168BB80551E6}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -813,7 +817,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -836,7 +840,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>22</v>
       </c>
@@ -844,7 +848,7 @@
         <v>26</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>37</v>
@@ -859,7 +863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="1" t="s">
@@ -878,11 +882,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>35</v>
@@ -897,7 +901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="1" t="s">
@@ -916,7 +920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -939,7 +943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -962,7 +966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>41</v>
       </c>
@@ -985,7 +989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>42</v>
       </c>
@@ -1008,7 +1012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="1" t="s">
@@ -1044,23 +1048,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89FF57BE-6DA6-9A46-A269-C97099FCCA20}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1086,7 +1090,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -1109,7 +1113,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>22</v>
       </c>
@@ -1117,7 +1121,7 @@
         <v>26</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>37</v>
@@ -1132,7 +1136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="1" t="s">
@@ -1151,11 +1155,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>35</v>
@@ -1170,7 +1174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="1" t="s">
@@ -1189,7 +1193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -1212,7 +1216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -1235,7 +1239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>41</v>
       </c>
@@ -1258,7 +1262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>42</v>
       </c>
@@ -1281,7 +1285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="1" t="s">
@@ -1300,12 +1304,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>38</v>
@@ -1323,7 +1327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="1" t="s">
@@ -1353,5 +1357,6 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: support description in field
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\irgen-rs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEDECE09-75B4-418D-A674-4D571F8861F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5FB1281-E21B-4B9B-8C90-F85476EF7517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{CE17D36E-8982-7C47-A020-5E6655990FA9}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="56">
   <si>
     <t>BLOCK</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -256,6 +256,10 @@
   </si>
   <si>
     <t>reserved0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg0.field0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -776,7 +780,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -838,6 +842,9 @@
       </c>
       <c r="G2" s="1" t="s">
         <v>34</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
refact: fix new example.xlsx
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Codes\irgen-rs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beribeli/Workspace/RustroverProjects/irgen-rs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5FB1281-E21B-4B9B-8C90-F85476EF7517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA5833B-93C2-6E4D-9651-6BDCD8093F01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{CE17D36E-8982-7C47-A020-5E6655990FA9}"/>
+    <workbookView xWindow="5180" yWindow="1900" windowWidth="23260" windowHeight="12460" activeTab="3" xr2:uid="{CE17D36E-8982-7C47-A020-5E6655990FA9}"/>
   </bookViews>
   <sheets>
     <sheet name="version" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="53">
   <si>
     <t>BLOCK</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -87,10 +87,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>WIDTH</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>ATTRIBUTE</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -216,14 +212,6 @@
   </si>
   <si>
     <t>[15:0]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TAG</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>VALUE</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -267,7 +255,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -653,61 +641,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{725A8A21-6CE1-5947-A0CB-208E9DE2092A}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="12.81640625" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
+    <row r="6" spans="1:5">
       <c r="B6" s="1"/>
     </row>
   </sheetData>
@@ -725,15 +701,15 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -744,29 +720,29 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -777,25 +753,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08ACDB31-7888-5646-9BBF-168BB80551E6}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="7.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -815,226 +790,193 @@
         <v>13</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="1">
+      <c r="E2" s="1" t="s">
         <v>32</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" s="1">
-        <v>8</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="1">
-        <v>8</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="1">
-        <v>8</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="1">
-        <v>8</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="E7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="1">
-        <v>32</v>
-      </c>
-      <c r="F7" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="1">
-        <v>32</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="E9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="1">
-        <v>32</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="B10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" s="1">
-        <v>16</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" s="1">
-        <v>16</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="1">
+        <v>43</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1053,25 +995,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89FF57BE-6DA6-9A46-A269-C97099FCCA20}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="7.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1091,265 +1032,226 @@
         <v>13</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="1">
+      <c r="E2" s="1" t="s">
         <v>32</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" s="1">
-        <v>8</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="1">
-        <v>8</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="1">
-        <v>8</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="1">
-        <v>8</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="E7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="1">
-        <v>32</v>
-      </c>
-      <c r="F7" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="1">
-        <v>32</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="E9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="1">
-        <v>32</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="B10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" s="1">
-        <v>16</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" s="1">
-        <v>16</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="1">
-        <v>16</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="1">
-        <v>16</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G13" s="1">
+        <v>43</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>